<commit_message>
Matchowanie autora po jednostce i tytule
</commit_message>
<xml_diff>
--- a/src/import_dyscyplin/tests/test1.xlsx
+++ b/src/import_dyscyplin/tests/test1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10319"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10309"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mpasternak/Programowanie/django-bpp/src/import_dyscyplin/tests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mpasternak/Programowanie/bpp/src/import_dyscyplin/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D9692D3-7009-F14B-BE74-CA06152C70DD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AECBAED4-BACF-4A42-81E3-5BE15324B48F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28520" windowHeight="12000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -371,7 +371,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Neutralne" xfId="1" builtinId="28"/>
+    <cellStyle name="Neutralny" xfId="1" builtinId="28"/>
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -653,13 +653,13 @@
   <dimension ref="A1:K1341"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="5"/>
-    <col min="2" max="2" width="22.1640625" style="4" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="22.1640625" style="4" customWidth="1"/>
     <col min="3" max="3" width="23.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.33203125" style="16" customWidth="1"/>
@@ -1274,7 +1274,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="11">
         <v>3</v>
       </c>
@@ -1303,7 +1303,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="11">
         <v>4</v>
       </c>
@@ -1332,7 +1332,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="11">
         <v>5</v>
       </c>
@@ -1361,7 +1361,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="11">
         <v>6</v>
       </c>
@@ -1390,7 +1390,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="11">
         <v>7</v>
       </c>
@@ -1428,7 +1428,7 @@
       <c r="F7" s="3"/>
       <c r="G7" s="12"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="11">
         <v>8</v>
       </c>
@@ -13565,7 +13565,7 @@
     </row>
     <row r="1341" spans="1:2" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <sortState ref="A2:I1373">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I1373">
     <sortCondition ref="G2:G1373"/>
     <sortCondition ref="F2:F1373"/>
     <sortCondition ref="C2:C1373"/>

</xml_diff>